<commit_message>
chore: upload demo file
</commit_message>
<xml_diff>
--- a/header_demo.xlsx
+++ b/header_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lzzzzzz/Desktop/Project.nosync/Fuck-Gridman/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D165DC88-A24B-3C4C-8136-9E265DF6D776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A57D0B-1FE3-4747-8B8E-2345B4615116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="38400" windowHeight="22100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="190">
   <si>
     <t>女</t>
   </si>
@@ -688,6 +688,14 @@
   </si>
   <si>
     <t>计算机01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>张三</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>李四</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1128,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1723,7 +1731,7 @@
         <v>40</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>130</v>
+        <v>189</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>1</v>
@@ -2335,7 +2343,7 @@
         <v>76</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>1</v>

</xml_diff>